<commit_message>
Added Priorites to the User Stories on Backlog
</commit_message>
<xml_diff>
--- a/documentation/Product Backlog.xlsx
+++ b/documentation/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de0b3ea1232571d3/Documents/School/Fall 24/InfoManage/MystiMedicare/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgain\OneDrive\Documents\School\info_man\MystiMedicare\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F2B70CE6-3504-48B0-8F7E-E8F97D216343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7EDB045-E917-4537-B6B2-2BEBBE84F099}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916C5772-1E77-456F-9210-7DD6969B61DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3135" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,18 +436,18 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,9 +461,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -475,7 +475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -489,7 +489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -503,9 +503,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -517,9 +517,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -531,9 +531,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -545,9 +545,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -559,9 +559,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -573,9 +573,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -587,9 +587,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added Missing user stories
</commit_message>
<xml_diff>
--- a/documentation/Product Backlog.xlsx
+++ b/documentation/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgain\OneDrive\Documents\School\info_man\MystiMedicare\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de0b3ea1232571d3/Documents/School/Fall 24/InfoManage/MystiMedicare/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916C5772-1E77-456F-9210-7DD6969B61DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{916C5772-1E77-456F-9210-7DD6969B61DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0E65515-33CD-496E-A087-39D638C6ED80}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Priority</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>so that I can perform custom queries</t>
+  </si>
+  <si>
+    <t>I want to edit patient information</t>
+  </si>
+  <si>
+    <t>so that I can update patient information</t>
+  </si>
+  <si>
+    <t>I want to search for patient visit information</t>
+  </si>
+  <si>
+    <t>so that I can see patient visit information</t>
+  </si>
+  <si>
+    <t>I want to search for patient appointment information</t>
+  </si>
+  <si>
+    <t>so that I can see patient appointment information</t>
   </si>
 </sst>
 </file>
@@ -433,21 +451,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,21 +479,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -483,27 +501,27 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -517,7 +535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -531,7 +549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -545,7 +563,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -559,51 +577,93 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
-    <sortCondition ref="A2:A19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D14">
+    <sortCondition ref="A1:A14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>